<commit_message>
limit the code size to SIMLOCK_NUM_CODES_MAX
</commit_message>
<xml_diff>
--- a/data_struct/simlock配.xlsx
+++ b/data_struct/simlock配.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="simlock配" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="G7" authorId="0">
@@ -36,7 +36,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>One item for a whole. Maybe sort it in building is a good choice.</t>
+          <t xml:space="preserve">One item for a whole. Maybe sort it in building is a good choice.</t>
         </r>
       </text>
     </comment>
@@ -49,7 +49,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>This should be set in runtime. Get data from nv.</t>
+          <t xml:space="preserve">This should be set in runtime. Get data from nv.</t>
         </r>
       </text>
     </comment>
@@ -62,7 +62,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>No this requirement by now.</t>
+          <t xml:space="preserve">No this requirement by now.</t>
         </r>
       </text>
     </comment>
@@ -73,7 +73,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="A20" authorId="0">
@@ -85,7 +85,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Less than 1536 bytes</t>
+          <t xml:space="preserve">Less than 1536 bytes</t>
         </r>
       </text>
     </comment>
@@ -98,7 +98,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Less than 128</t>
+          <t xml:space="preserve">Less than 128</t>
         </r>
       </text>
     </comment>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="60">
   <si>
     <t xml:space="preserve">field</t>
   </si>
@@ -226,52 +226,58 @@
     <t xml:space="preserve">reserved</t>
   </si>
   <si>
+    <t xml:space="preserve">slot_count(&lt;SIMLOCK_SLOT_NUM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(slot_count*slot_config_data) bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsa_sig_magic=0x55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsa_sig_len</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsa_sig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slot_config_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slot_config_data_magic=0x5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simlock_category_enum_count(&lt;=SIMLOCK_CATEGORY_3GPP2_RUIM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(simlock_category_enum_count*simlock_category_data) bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simlock_category_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simlock_category_data_magic=0xAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auto_lock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_blacklist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">retry times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code_data: contain simlock_category_enum_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">magic</t>
+  </si>
+  <si>
     <t xml:space="preserve">slot_count</t>
   </si>
   <si>
-    <t xml:space="preserve">(slot_count*slot_config_data) bytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsa_sig_magic=0x55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsa_sig_len</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsa_sig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">slot_config_data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">slot_config_data_magic=0x5A</t>
-  </si>
-  <si>
     <t xml:space="preserve">simlock_category_enum_count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(simlock_category_enum_count*simlock_category_data) bytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">simlock_category_data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">simlock_category_data_magic=0xAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">auto_lock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_blacklist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">retry times</t>
-  </si>
-  <si>
-    <t xml:space="preserve">code_data: contain simlock_category_enum_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">magic</t>
   </si>
   <si>
     <t xml:space="preserve">code_data_size</t>
@@ -698,17 +704,17 @@
   </sheetPr>
   <dimension ref="A1:G164"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.75"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1947,7 +1953,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1963,21 +1969,21 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="29" width="51.4336734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="29" width="51.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,7 +2416,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2425,13 +2431,13 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2514,7 +2520,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="32" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B7" s="32"/>
       <c r="C7" s="35" t="s">
@@ -2584,7 +2590,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -2692,7 +2698,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="32" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -2704,7 +2710,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="32" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -2716,7 +2722,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="33" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B25" s="33"/>
       <c r="C25" s="33"/>
@@ -2776,7 +2782,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>